<commit_message>
Corrected the question on who completed the questionnaire.
</commit_message>
<xml_diff>
--- a/Metadata/TBStigmaHouseholdSurvey_DataDictionary_2022-08-05.xlsx
+++ b/Metadata/TBStigmaHouseholdSurvey_DataDictionary_2022-08-05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://foundationcoza-my.sharepoint.com/personal/freedomm_foundation_co_za/Documents/Documents/Projects/TB Stigma/TB-Stigma/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C952038-6138-43D8-AB1C-6B4340383618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{8C952038-6138-43D8-AB1C-6B4340383618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1670C101-4F57-4558-89FA-8351F7A9FD97}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBStigmaHouseholdSurvey_DataDic" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TBStigmaHouseholdSurvey_DataDic!$A$1:$T$1001</definedName>
   </definedNames>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -7428,7 +7428,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8265,11 +8265,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A967" sqref="A967:B994"/>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16388,7 +16388,7 @@
       </c>
     </row>
     <row r="295" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A295">
+      <c r="B295">
         <v>1</v>
       </c>
       <c r="C295" t="s">
@@ -35901,7 +35901,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1001"/>
+  <autoFilter ref="A1:T1001" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>